<commit_message>
Merge text and code false postives/negatives
</commit_message>
<xml_diff>
--- a/metric-selection/fp+fn/f_text.xlsx
+++ b/metric-selection/fp+fn/f_text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\github\sotorrent\r-scripts\metric-selection\fp+fn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/git/github/sotorrent/r-scripts/metric-selection/fp+fn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB08913D-3650-4324-AEDE-22D7BE14A8C1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1BD627-294E-6744-9402-5C66F0AC6694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="8820" windowWidth="27645" windowHeight="16935" xr2:uid="{F7682DBE-4F8B-B341-821A-0A12D1D8B3A2}"/>
+    <workbookView xWindow="7600" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{F7682DBE-4F8B-B341-821A-0A12D1D8B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,17 +453,17 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>122291</v>
       </c>
@@ -489,7 +489,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2579869</v>
       </c>
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2749893</v>
       </c>
@@ -511,7 +511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3872793</v>
       </c>
@@ -522,7 +522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3920776</v>
       </c>
@@ -533,7 +533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4696621</v>
       </c>
@@ -544,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7016109</v>
       </c>
@@ -555,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7488478</v>
       </c>
@@ -566,7 +566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7837122</v>
       </c>
@@ -577,7 +577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7893947</v>
       </c>
@@ -588,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9037142</v>
       </c>
@@ -599,7 +599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10463373</v>
       </c>
@@ -610,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11077528</v>
       </c>
@@ -619,7 +619,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12633603</v>
       </c>
@@ -630,7 +630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13081285</v>
       </c>
@@ -641,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14393231</v>
       </c>
@@ -650,7 +650,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15037082</v>
       </c>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15119106</v>
       </c>
@@ -670,7 +670,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>15372744</v>
       </c>
@@ -679,7 +679,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>16581752</v>
       </c>
@@ -690,7 +690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>17158055</v>
       </c>
@@ -699,7 +699,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>18932575</v>
       </c>
@@ -710,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>19612096</v>
       </c>
@@ -724,7 +724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20038558</v>
       </c>
@@ -738,7 +738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20586684</v>
       </c>
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20786845</v>
       </c>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20965995</v>
       </c>
@@ -769,7 +769,7 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>21120863</v>
       </c>
@@ -780,7 +780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23217455</v>
       </c>
@@ -791,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>24848884</v>
       </c>
@@ -800,7 +800,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>25160608</v>
       </c>
@@ -814,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>25488162</v>
       </c>
@@ -825,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>25547131</v>
       </c>
@@ -839,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>25871278</v>
       </c>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>26446315</v>
       </c>
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>26953938</v>
       </c>
@@ -869,7 +869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>27803362</v>
       </c>
@@ -877,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>27841344</v>
       </c>
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>27874548</v>
       </c>
@@ -899,7 +899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>27971168</v>
       </c>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>28623462</v>
       </c>
@@ -918,7 +918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>28785113</v>
       </c>
@@ -926,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>29071745</v>
       </c>
@@ -937,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>29443655</v>
       </c>
@@ -951,7 +951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>30355942</v>
       </c>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>31054664</v>
       </c>
@@ -970,7 +970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>31738071</v>
       </c>
@@ -981,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>32205729</v>
       </c>
@@ -995,7 +995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>32801275</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>33678952</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>33685540</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>33813930</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>35398661</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>36741782</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>37196630</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>37876734</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>38136787</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>39016820</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>39552029</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>41480290</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>42237737</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>44149391</v>
       </c>
@@ -1154,8 +1154,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E63" xr:uid="{9170F7C2-FC38-DD4C-82BE-4AC2A21024B0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E63">
-      <sortCondition ref="A1:A32"/>
+    <sortState ref="A2:E63">
+      <sortCondition ref="A1:A63"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>